<commit_message>
Linked to namegen, started several new modules
</commit_message>
<xml_diff>
--- a/files/Character Sheet (Template).xlsx
+++ b/files/Character Sheet (Template).xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Character" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Skills" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Spells" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Equipment" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>DundTools</t>
   </si>
@@ -98,6 +103,9 @@
   </si>
   <si>
     <t xml:space="preserve">Hit Dice:</t>
+  </si>
+  <si>
+    <t>Rage</t>
   </si>
   <si>
     <t xml:space="preserve">Death Saves</t>
@@ -517,7 +525,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="65">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -582,7 +590,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="3" numFmtId="0" xfId="0" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -671,14 +678,13 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
       <protection hidden="0" locked="1"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="15" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf fontId="2" fillId="0" borderId="16" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="2" fillId="9" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1351,28 +1357,28 @@
       <c r="C8" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="24"/>
+      <c r="D8" s="8"/>
       <c r="F8" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="24"/>
+      <c r="G8" s="8"/>
       <c r="H8" s="4"/>
       <c r="I8" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="24"/>
+      <c r="J8" s="8"/>
       <c r="L8" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="24"/>
+      <c r="M8" s="8"/>
       <c r="O8" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="P8" s="24"/>
+      <c r="P8" s="8"/>
       <c r="R8" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="S8" s="24"/>
+      <c r="S8" s="8"/>
       <c r="U8" s="19"/>
       <c r="V8" s="19"/>
     </row>
@@ -1398,14 +1404,14 @@
       <c r="I11" s="17"/>
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
-      <c r="M11" s="25"/>
+      <c r="M11" s="24"/>
       <c r="N11" s="17" t="s">
         <v>23</v>
       </c>
       <c r="O11" s="17"/>
       <c r="P11" s="17"/>
       <c r="Q11" s="17"/>
-      <c r="R11" s="25"/>
+      <c r="R11" s="24"/>
       <c r="S11" s="17" t="s">
         <v>24</v>
       </c>
@@ -1424,14 +1430,14 @@
       <c r="I12" s="17"/>
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
-      <c r="M12" s="25"/>
+      <c r="M12" s="24"/>
       <c r="N12" s="17" t="s">
         <v>26</v>
       </c>
       <c r="O12" s="17"/>
       <c r="P12" s="17"/>
       <c r="Q12" s="17"/>
-      <c r="R12" s="25"/>
+      <c r="R12" s="24"/>
       <c r="S12" s="17"/>
       <c r="T12" s="17"/>
       <c r="U12" s="17"/>
@@ -1444,18 +1450,21 @@
       <c r="D15" s="17"/>
       <c r="E15" s="19"/>
       <c r="F15" s="19"/>
+      <c r="H15" s="17" t="s">
+        <v>28</v>
+      </c>
       <c r="J15" s="17" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K15" s="17"/>
       <c r="L15" s="17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M15" s="19"/>
       <c r="N15" s="19"/>
       <c r="O15" s="19"/>
       <c r="Q15" s="17" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="R15" s="17"/>
       <c r="S15" s="17"/>
@@ -1464,346 +1473,367 @@
       <c r="V15" s="17"/>
     </row>
     <row r="16" ht="14.25">
+      <c r="H16" s="19"/>
       <c r="J16" s="17"/>
       <c r="K16" s="17"/>
       <c r="L16" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M16" s="19"/>
       <c r="N16" s="19"/>
       <c r="O16" s="19"/>
-      <c r="Q16" s="26"/>
-      <c r="R16" s="26"/>
-      <c r="S16" s="26"/>
-      <c r="T16" s="26"/>
-      <c r="U16" s="26"/>
-      <c r="V16" s="26"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25"/>
+      <c r="T16" s="25"/>
+      <c r="U16" s="25"/>
+      <c r="V16" s="25"/>
     </row>
     <row r="17" ht="14.25">
-      <c r="Q17" s="26"/>
-      <c r="R17" s="26"/>
-      <c r="S17" s="26"/>
-      <c r="T17" s="26"/>
-      <c r="U17" s="26"/>
-      <c r="V17" s="26"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="25"/>
+      <c r="V17" s="25"/>
     </row>
     <row r="18" ht="14.25">
-      <c r="Q18" s="26"/>
-      <c r="R18" s="26"/>
-      <c r="S18" s="26"/>
-      <c r="T18" s="26"/>
-      <c r="U18" s="26"/>
-      <c r="V18" s="26"/>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="25"/>
+      <c r="S18" s="25"/>
+      <c r="T18" s="25"/>
+      <c r="U18" s="25"/>
+      <c r="V18" s="25"/>
     </row>
     <row r="19" ht="14.25">
       <c r="C19" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
-      <c r="G19" s="27"/>
+      <c r="G19" s="26"/>
       <c r="J19" s="17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K19" s="17"/>
       <c r="L19" s="17"/>
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
       <c r="O19" s="17"/>
-      <c r="Q19" s="26"/>
-      <c r="R19" s="26"/>
-      <c r="S19" s="26"/>
-      <c r="T19" s="26"/>
-      <c r="U19" s="26"/>
-      <c r="V19" s="26"/>
+      <c r="Q19" s="25"/>
+      <c r="R19" s="25"/>
+      <c r="S19" s="25"/>
+      <c r="T19" s="25"/>
+      <c r="U19" s="25"/>
+      <c r="V19" s="25"/>
     </row>
     <row r="20" ht="14.25">
-      <c r="C20" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" s="29"/>
-      <c r="E20" s="30"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="31"/>
+      <c r="C20" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="28"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="30"/>
       <c r="J20" s="19"/>
       <c r="K20" s="19"/>
       <c r="L20" s="19"/>
       <c r="M20" s="19"/>
       <c r="N20" s="19"/>
       <c r="O20" s="19"/>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="26"/>
-      <c r="S20" s="26"/>
-      <c r="T20" s="26"/>
-      <c r="U20" s="26"/>
-      <c r="V20" s="26"/>
+      <c r="Q20" s="25"/>
+      <c r="R20" s="25"/>
+      <c r="S20" s="25"/>
+      <c r="T20" s="25"/>
+      <c r="U20" s="25"/>
+      <c r="V20" s="25"/>
     </row>
     <row r="21" ht="14.25">
-      <c r="C21" s="32"/>
-      <c r="D21" s="33"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="32"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="34"/>
+      <c r="G21" s="33"/>
       <c r="J21" s="19"/>
       <c r="K21" s="19"/>
       <c r="L21" s="19"/>
       <c r="M21" s="19"/>
       <c r="N21" s="19"/>
       <c r="O21" s="19"/>
-      <c r="Q21" s="26"/>
-      <c r="R21" s="26"/>
-      <c r="S21" s="26"/>
-      <c r="T21" s="26"/>
-      <c r="U21" s="26"/>
-      <c r="V21" s="26"/>
+      <c r="Q21" s="25"/>
+      <c r="R21" s="25"/>
+      <c r="S21" s="25"/>
+      <c r="T21" s="25"/>
+      <c r="U21" s="25"/>
+      <c r="V21" s="25"/>
     </row>
     <row r="22" ht="14.25">
-      <c r="C22" s="32"/>
-      <c r="D22" s="33"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="32"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="34"/>
+      <c r="G22" s="33"/>
       <c r="J22" s="19"/>
       <c r="K22" s="19"/>
       <c r="L22" s="19"/>
       <c r="M22" s="19"/>
       <c r="N22" s="19"/>
       <c r="O22" s="19"/>
-      <c r="Q22" s="26"/>
-      <c r="R22" s="26"/>
-      <c r="S22" s="26"/>
-      <c r="T22" s="26"/>
-      <c r="U22" s="26"/>
-      <c r="V22" s="26"/>
+      <c r="Q22" s="25"/>
+      <c r="R22" s="25"/>
+      <c r="S22" s="25"/>
+      <c r="T22" s="25"/>
+      <c r="U22" s="25"/>
+      <c r="V22" s="25"/>
     </row>
     <row r="23" ht="14.25">
-      <c r="C23" s="32"/>
-      <c r="D23" s="33"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="32"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="34"/>
+      <c r="G23" s="33"/>
       <c r="J23" s="19"/>
       <c r="K23" s="19"/>
       <c r="L23" s="19"/>
       <c r="M23" s="19"/>
       <c r="N23" s="19"/>
       <c r="O23" s="19"/>
-      <c r="Q23" s="26"/>
-      <c r="R23" s="26"/>
-      <c r="S23" s="26"/>
-      <c r="T23" s="26"/>
-      <c r="U23" s="26"/>
-      <c r="V23" s="26"/>
+      <c r="Q23" s="25"/>
+      <c r="R23" s="25"/>
+      <c r="S23" s="25"/>
+      <c r="T23" s="25"/>
+      <c r="U23" s="25"/>
+      <c r="V23" s="25"/>
     </row>
     <row r="24" ht="14.25">
-      <c r="C24" s="32"/>
-      <c r="D24" s="33"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="32"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="G24" s="34"/>
+      <c r="G24" s="33"/>
       <c r="J24" s="19"/>
       <c r="K24" s="19"/>
       <c r="L24" s="19"/>
       <c r="M24" s="19"/>
       <c r="N24" s="19"/>
       <c r="O24" s="19"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="26"/>
-      <c r="S24" s="26"/>
-      <c r="T24" s="26"/>
-      <c r="U24" s="26"/>
-      <c r="V24" s="26"/>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="25"/>
+      <c r="S24" s="25"/>
+      <c r="T24" s="25"/>
+      <c r="U24" s="25"/>
+      <c r="V24" s="25"/>
     </row>
     <row r="25" ht="14.25">
-      <c r="C25" s="32"/>
-      <c r="D25" s="33"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="32"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
-      <c r="G25" s="34"/>
-      <c r="Q25" s="26"/>
-      <c r="R25" s="26"/>
-      <c r="S25" s="26"/>
-      <c r="T25" s="26"/>
-      <c r="U25" s="26"/>
-      <c r="V25" s="26"/>
+      <c r="G25" s="33"/>
+      <c r="Q25" s="25"/>
+      <c r="R25" s="25"/>
+      <c r="S25" s="25"/>
+      <c r="T25" s="25"/>
+      <c r="U25" s="25"/>
+      <c r="V25" s="25"/>
     </row>
     <row r="26" ht="14.25">
-      <c r="C26" s="35"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="38"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="37"/>
       <c r="J26" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K26" s="17"/>
       <c r="L26" s="17"/>
       <c r="M26" s="17"/>
       <c r="N26" s="17"/>
       <c r="O26" s="17"/>
-      <c r="Q26" s="26"/>
-      <c r="R26" s="26"/>
-      <c r="S26" s="26"/>
-      <c r="T26" s="26"/>
-      <c r="U26" s="26"/>
-      <c r="V26" s="26"/>
+      <c r="Q26" s="25"/>
+      <c r="R26" s="25"/>
+      <c r="S26" s="25"/>
+      <c r="T26" s="25"/>
+      <c r="U26" s="25"/>
+      <c r="V26" s="25"/>
     </row>
     <row r="27" ht="14.25">
-      <c r="C27" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" s="29"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="31"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="30"/>
-      <c r="L27" s="31"/>
-      <c r="M27" s="39"/>
-      <c r="N27" s="30"/>
-      <c r="O27" s="31"/>
-      <c r="Q27" s="26"/>
-      <c r="R27" s="26"/>
-      <c r="S27" s="26"/>
-      <c r="T27" s="26"/>
-      <c r="U27" s="26"/>
-      <c r="V27" s="26"/>
+      <c r="C27" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="28"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="30"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="30"/>
+      <c r="M27" s="38"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="30"/>
+      <c r="Q27" s="25"/>
+      <c r="R27" s="25"/>
+      <c r="S27" s="25"/>
+      <c r="T27" s="25"/>
+      <c r="U27" s="25"/>
+      <c r="V27" s="25"/>
     </row>
     <row r="28" ht="14.25">
-      <c r="C28" s="32"/>
-      <c r="D28" s="33"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="32"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="34"/>
-      <c r="J28" s="40"/>
+      <c r="G28" s="33"/>
+      <c r="J28" s="39"/>
       <c r="K28" s="4"/>
-      <c r="L28" s="34"/>
-      <c r="M28" s="40"/>
+      <c r="L28" s="33"/>
+      <c r="M28" s="39"/>
       <c r="N28" s="4"/>
-      <c r="O28" s="34"/>
-      <c r="Q28" s="26"/>
-      <c r="R28" s="26"/>
-      <c r="S28" s="26"/>
-      <c r="T28" s="26"/>
-      <c r="U28" s="26"/>
-      <c r="V28" s="26"/>
+      <c r="O28" s="33"/>
+      <c r="Q28" s="25"/>
+      <c r="R28" s="25"/>
+      <c r="S28" s="25"/>
+      <c r="T28" s="25"/>
+      <c r="U28" s="25"/>
+      <c r="V28" s="25"/>
     </row>
     <row r="29" ht="14.25">
-      <c r="C29" s="35"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="38"/>
-      <c r="J29" s="40"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="33"/>
+      <c r="J29" s="39"/>
       <c r="K29" s="4"/>
-      <c r="L29" s="34"/>
-      <c r="M29" s="40"/>
+      <c r="L29" s="33"/>
+      <c r="M29" s="39"/>
       <c r="N29" s="4"/>
-      <c r="O29" s="34"/>
-      <c r="Q29" s="26"/>
-      <c r="R29" s="26"/>
-      <c r="S29" s="26"/>
-      <c r="T29" s="26"/>
-      <c r="U29" s="26"/>
-      <c r="V29" s="26"/>
+      <c r="O29" s="33"/>
+      <c r="Q29" s="25"/>
+      <c r="R29" s="25"/>
+      <c r="S29" s="25"/>
+      <c r="T29" s="25"/>
+      <c r="U29" s="25"/>
+      <c r="V29" s="25"/>
     </row>
     <row r="30" ht="14.25">
-      <c r="C30" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="29"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="31"/>
-      <c r="J30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="33"/>
+      <c r="J30" s="39"/>
       <c r="K30" s="4"/>
-      <c r="L30" s="34"/>
-      <c r="M30" s="40"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="39"/>
       <c r="N30" s="4"/>
-      <c r="O30" s="34"/>
-      <c r="Q30" s="26"/>
-      <c r="R30" s="26"/>
-      <c r="S30" s="26"/>
-      <c r="T30" s="26"/>
-      <c r="U30" s="26"/>
-      <c r="V30" s="26"/>
+      <c r="O30" s="33"/>
+      <c r="Q30" s="25"/>
+      <c r="R30" s="25"/>
+      <c r="S30" s="25"/>
+      <c r="T30" s="25"/>
+      <c r="U30" s="25"/>
+      <c r="V30" s="25"/>
     </row>
     <row r="31" ht="14.25">
       <c r="C31" s="41"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="34"/>
-      <c r="J31" s="40"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="36"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="37"/>
+      <c r="J31" s="39"/>
       <c r="K31" s="4"/>
-      <c r="L31" s="34"/>
-      <c r="M31" s="40"/>
+      <c r="L31" s="33"/>
+      <c r="M31" s="39"/>
       <c r="N31" s="4"/>
-      <c r="O31" s="34"/>
-      <c r="Q31" s="26"/>
-      <c r="R31" s="26"/>
-      <c r="S31" s="26"/>
-      <c r="T31" s="26"/>
-      <c r="U31" s="26"/>
-      <c r="V31" s="26"/>
+      <c r="O31" s="33"/>
+      <c r="Q31" s="25"/>
+      <c r="R31" s="25"/>
+      <c r="S31" s="25"/>
+      <c r="T31" s="25"/>
+      <c r="U31" s="25"/>
+      <c r="V31" s="25"/>
     </row>
     <row r="32" ht="14.25">
-      <c r="C32" s="41"/>
+      <c r="C32" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="28"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="34"/>
-      <c r="J32" s="40"/>
+      <c r="G32" s="33"/>
+      <c r="J32" s="39"/>
       <c r="K32" s="4"/>
-      <c r="L32" s="34"/>
-      <c r="M32" s="40"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="39"/>
       <c r="N32" s="4"/>
-      <c r="O32" s="34"/>
-      <c r="Q32" s="26"/>
-      <c r="R32" s="26"/>
-      <c r="S32" s="26"/>
-      <c r="T32" s="26"/>
-      <c r="U32" s="26"/>
-      <c r="V32" s="26"/>
+      <c r="O32" s="33"/>
+      <c r="Q32" s="25"/>
+      <c r="R32" s="25"/>
+      <c r="S32" s="25"/>
+      <c r="T32" s="25"/>
+      <c r="U32" s="25"/>
+      <c r="V32" s="25"/>
     </row>
     <row r="33" ht="14.25">
-      <c r="C33" s="41"/>
+      <c r="C33" s="40"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="34"/>
-      <c r="J33" s="40"/>
+      <c r="G33" s="33"/>
+      <c r="J33" s="39"/>
       <c r="K33" s="4"/>
-      <c r="L33" s="34"/>
-      <c r="M33" s="40"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="39"/>
       <c r="N33" s="4"/>
-      <c r="O33" s="34"/>
-      <c r="Q33" s="26"/>
-      <c r="R33" s="26"/>
-      <c r="S33" s="26"/>
-      <c r="T33" s="26"/>
-      <c r="U33" s="26"/>
-      <c r="V33" s="26"/>
+      <c r="O33" s="33"/>
+      <c r="Q33" s="25"/>
+      <c r="R33" s="25"/>
+      <c r="S33" s="25"/>
+      <c r="T33" s="25"/>
+      <c r="U33" s="25"/>
+      <c r="V33" s="25"/>
     </row>
     <row r="34" ht="14.25">
-      <c r="C34" s="42"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="38"/>
-      <c r="J34" s="44"/>
-      <c r="K34" s="37"/>
-      <c r="L34" s="38"/>
-      <c r="M34" s="44"/>
-      <c r="N34" s="37"/>
-      <c r="O34" s="38"/>
-      <c r="Q34" s="26"/>
-      <c r="R34" s="26"/>
-      <c r="S34" s="26"/>
-      <c r="T34" s="26"/>
-      <c r="U34" s="26"/>
-      <c r="V34" s="26"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="33"/>
+      <c r="J34" s="43"/>
+      <c r="K34" s="36"/>
+      <c r="L34" s="37"/>
+      <c r="M34" s="43"/>
+      <c r="N34" s="36"/>
+      <c r="O34" s="37"/>
+      <c r="Q34" s="25"/>
+      <c r="R34" s="25"/>
+      <c r="S34" s="25"/>
+      <c r="T34" s="25"/>
+      <c r="U34" s="25"/>
+      <c r="V34" s="25"/>
+    </row>
+    <row r="35" ht="14.25">
+      <c r="C35" s="40"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="33"/>
+    </row>
+    <row r="36" ht="14.25">
+      <c r="C36" s="40"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="33"/>
+    </row>
+    <row r="37" ht="14.25">
+      <c r="C37" s="41"/>
+      <c r="D37" s="42"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
+      <c r="G37" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="84">
+  <mergeCells count="87">
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="J2:K2"/>
@@ -1872,13 +1902,13 @@
     <mergeCell ref="E29:G29"/>
     <mergeCell ref="J29:L29"/>
     <mergeCell ref="M29:O29"/>
-    <mergeCell ref="C30:D30"/>
     <mergeCell ref="E30:G30"/>
     <mergeCell ref="J30:L30"/>
     <mergeCell ref="M30:O30"/>
     <mergeCell ref="E31:G31"/>
     <mergeCell ref="J31:L31"/>
     <mergeCell ref="M31:O31"/>
+    <mergeCell ref="C32:D32"/>
     <mergeCell ref="E32:G32"/>
     <mergeCell ref="J32:L32"/>
     <mergeCell ref="M32:O32"/>
@@ -1888,6 +1918,9 @@
     <mergeCell ref="E34:G34"/>
     <mergeCell ref="J34:L34"/>
     <mergeCell ref="M34:O34"/>
+    <mergeCell ref="E35:G35"/>
+    <mergeCell ref="E36:G36"/>
+    <mergeCell ref="E37:G37"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
@@ -1919,81 +1952,81 @@
       </c>
     </row>
     <row r="3">
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="46"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="48" t="s">
+      <c r="D3" s="45"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="49"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="50" t="s">
+      <c r="G3" s="48"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="51"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="52" t="s">
+      <c r="J3" s="50"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="53"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="54" t="s">
+      <c r="M3" s="52"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="47"/>
-      <c r="R3" s="56" t="s">
+      <c r="P3" s="54"/>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="S3" s="57"/>
-      <c r="T3" s="47"/>
+      <c r="S3" s="56"/>
+      <c r="T3" s="46"/>
       <c r="U3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="V3" s="27"/>
+      <c r="V3" s="26"/>
     </row>
     <row r="4">
-      <c r="C4" s="39"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="31"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="31"/>
-      <c r="Q4" s="47"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="31"/>
-      <c r="T4" s="47"/>
-      <c r="U4" s="39"/>
-      <c r="V4" s="31"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="38"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="46"/>
+      <c r="R4" s="38"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="46"/>
+      <c r="U4" s="38"/>
+      <c r="V4" s="30"/>
     </row>
     <row r="5">
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="F5" s="19"/>
       <c r="G5" s="19"/>
-      <c r="H5" s="58"/>
+      <c r="H5" s="57"/>
       <c r="I5" s="19"/>
       <c r="J5" s="19"/>
-      <c r="K5" s="58"/>
+      <c r="K5" s="57"/>
       <c r="L5" s="19"/>
       <c r="M5" s="19"/>
-      <c r="N5" s="58"/>
+      <c r="N5" s="57"/>
       <c r="O5" s="19"/>
       <c r="P5" s="19"/>
-      <c r="Q5" s="58"/>
+      <c r="Q5" s="57"/>
       <c r="R5" s="19"/>
       <c r="S5" s="19"/>
-      <c r="T5" s="58"/>
+      <c r="T5" s="57"/>
       <c r="U5" s="19"/>
       <c r="V5" s="19"/>
     </row>
@@ -2001,57 +2034,57 @@
       <c r="C6" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="47"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="46"/>
       <c r="F6" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="24"/>
+      <c r="G6" s="58"/>
       <c r="H6" s="59"/>
       <c r="I6" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="24"/>
-      <c r="K6" s="47"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="46"/>
       <c r="L6" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="24"/>
-      <c r="N6" s="47"/>
+      <c r="M6" s="58"/>
+      <c r="N6" s="46"/>
       <c r="O6" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="47"/>
+      <c r="P6" s="58"/>
+      <c r="Q6" s="46"/>
       <c r="R6" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="S6" s="24"/>
-      <c r="T6" s="58"/>
+      <c r="S6" s="58"/>
+      <c r="T6" s="57"/>
       <c r="U6" s="19"/>
-      <c r="V6" s="38"/>
+      <c r="V6" s="37"/>
     </row>
     <row r="9">
       <c r="B9" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
       <c r="G9" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
       <c r="M9" s="60" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N9" s="60"/>
       <c r="O9" s="60"/>
@@ -2062,378 +2095,450 @@
       <c r="T9" s="60"/>
     </row>
     <row r="10">
-      <c r="B10" s="61"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="11" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="11"/>
-      <c r="E10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" s="63"/>
-      <c r="J10" s="62"/>
+      <c r="E10" s="19" t="e">
+        <f>IF(B10="X",VALUE(D6)+VALUE(U4),VALUE(D6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G10" s="19"/>
+      <c r="H10" s="61" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="61"/>
+      <c r="J10" s="19" t="e">
+        <f>IF(G10="X",VALUE(G6)+VALUE(U4),VALUE(G6))</f>
+        <v>#VALUE!</v>
+      </c>
       <c r="M10" s="60" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="N10" s="60"/>
       <c r="O10" s="60" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="P10" s="60"/>
       <c r="Q10" s="60" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="R10" s="60"/>
       <c r="S10" s="60" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="T10" s="60"/>
     </row>
     <row r="11">
-      <c r="B11" s="61"/>
-      <c r="C11" s="63" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="63"/>
-      <c r="E11" s="62"/>
-      <c r="G11" s="62"/>
-      <c r="H11" s="64" t="s">
-        <v>47</v>
-      </c>
-      <c r="I11" s="64"/>
-      <c r="J11" s="62"/>
-      <c r="M11" s="65"/>
-      <c r="N11" s="65"/>
-      <c r="O11" s="65"/>
-      <c r="P11" s="65"/>
-      <c r="Q11" s="65"/>
-      <c r="R11" s="65"/>
-      <c r="S11" s="65"/>
-      <c r="T11" s="65"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="19" t="e">
+        <f>IF(B11="X",VALUE(G6)+VALUE(U4),VALUE(G6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G11" s="19"/>
+      <c r="H11" s="62" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="62"/>
+      <c r="J11" s="19" t="e">
+        <f>IF(G11="X",VALUE(P6)+VALUE(U4),VALUE(P6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M11" s="63"/>
+      <c r="N11" s="63"/>
+      <c r="O11" s="63"/>
+      <c r="P11" s="63"/>
+      <c r="Q11" s="63"/>
+      <c r="R11" s="63"/>
+      <c r="S11" s="63"/>
+      <c r="T11" s="63"/>
     </row>
     <row r="12">
-      <c r="B12" s="61"/>
-      <c r="C12" s="66" t="s">
+      <c r="B12" s="17"/>
+      <c r="C12" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="66"/>
-      <c r="E12" s="62"/>
-      <c r="G12" s="62"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="19" t="e">
+        <f>IF(B12="X",VALUE(J6)+VALUE(U4),VALUE(D6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G12" s="19"/>
       <c r="H12" s="14" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I12" s="14"/>
-      <c r="J12" s="62"/>
-      <c r="M12" s="65"/>
-      <c r="N12" s="65"/>
-      <c r="O12" s="65"/>
-      <c r="P12" s="65"/>
-      <c r="Q12" s="65"/>
-      <c r="R12" s="65"/>
-      <c r="S12" s="65"/>
-      <c r="T12" s="65"/>
+      <c r="J12" s="19" t="e">
+        <f>IF(G12="X",VALUE(M6)+VALUE(U4),VALUE(M6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="63"/>
+      <c r="P12" s="63"/>
+      <c r="Q12" s="63"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="63"/>
+      <c r="T12" s="63"/>
     </row>
     <row r="13">
-      <c r="B13" s="61"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D13" s="14"/>
-      <c r="E13" s="62"/>
-      <c r="G13" s="62"/>
+      <c r="E13" s="19" t="e">
+        <f>IF(B13="X",VALUE(M6)+VALUE(U4),VALUE(M6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G13" s="19"/>
       <c r="H13" s="11" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="I13" s="11"/>
-      <c r="J13" s="62"/>
-      <c r="M13" s="65"/>
-      <c r="N13" s="65"/>
-      <c r="O13" s="65"/>
-      <c r="P13" s="65"/>
-      <c r="Q13" s="65"/>
-      <c r="R13" s="65"/>
-      <c r="S13" s="65"/>
-      <c r="T13" s="65"/>
+      <c r="J13" s="19" t="e">
+        <f>IF(G13="X",VALUE(D6)+VALUE(U4),VALUE(D6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M13" s="63"/>
+      <c r="N13" s="63"/>
+      <c r="O13" s="63"/>
+      <c r="P13" s="63"/>
+      <c r="Q13" s="63"/>
+      <c r="R13" s="63"/>
+      <c r="S13" s="63"/>
+      <c r="T13" s="63"/>
     </row>
     <row r="14">
-      <c r="B14" s="61"/>
-      <c r="C14" s="64" t="s">
+      <c r="B14" s="17"/>
+      <c r="C14" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="64"/>
-      <c r="E14" s="62"/>
-      <c r="G14" s="62"/>
-      <c r="H14" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="I14" s="17"/>
-      <c r="J14" s="62"/>
-      <c r="M14" s="65"/>
-      <c r="N14" s="65"/>
-      <c r="O14" s="65"/>
-      <c r="P14" s="65"/>
-      <c r="Q14" s="65"/>
-      <c r="R14" s="65"/>
-      <c r="S14" s="65"/>
-      <c r="T14" s="65"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="19" t="e">
+        <f>IF(B14="X",VALUE(P6)+VALUE(U4),VALUE(P6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G14" s="19"/>
+      <c r="H14" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" s="16"/>
+      <c r="J14" s="19" t="e">
+        <f>IF(G14="X",VALUE(S6)+VALUE(U4),VALUE(S6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M14" s="63"/>
+      <c r="N14" s="63"/>
+      <c r="O14" s="63"/>
+      <c r="P14" s="63"/>
+      <c r="Q14" s="63"/>
+      <c r="R14" s="63"/>
+      <c r="S14" s="63"/>
+      <c r="T14" s="63"/>
     </row>
     <row r="15">
-      <c r="B15" s="61"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="16" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="16"/>
-      <c r="E15" s="62"/>
-      <c r="G15" s="62"/>
+      <c r="E15" s="19" t="e">
+        <f>IF(B15="X",VALUE(S6)+VALUE(U4),VALUE(S6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G15" s="19"/>
       <c r="H15" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="I15" s="14"/>
-      <c r="J15" s="62"/>
-      <c r="M15" s="65"/>
-      <c r="N15" s="65"/>
-      <c r="O15" s="65"/>
-      <c r="P15" s="65"/>
-      <c r="Q15" s="65"/>
-      <c r="R15" s="65"/>
-      <c r="S15" s="65"/>
-      <c r="T15" s="65"/>
+      <c r="J15" s="19" t="e">
+        <f>IF(G15="X",VALUE(M6)+VALUE(U4),VALUE(M6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M15" s="63"/>
+      <c r="N15" s="63"/>
+      <c r="O15" s="63"/>
+      <c r="P15" s="63"/>
+      <c r="Q15" s="63"/>
+      <c r="R15" s="63"/>
+      <c r="S15" s="63"/>
+      <c r="T15" s="63"/>
     </row>
     <row r="16">
-      <c r="G16" s="62"/>
-      <c r="H16" s="64" t="s">
-        <v>52</v>
-      </c>
-      <c r="I16" s="64"/>
-      <c r="J16" s="62"/>
-      <c r="M16" s="65"/>
-      <c r="N16" s="65"/>
-      <c r="O16" s="65"/>
-      <c r="P16" s="65"/>
-      <c r="Q16" s="65"/>
-      <c r="R16" s="65"/>
-      <c r="S16" s="65"/>
-      <c r="T16" s="65"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="62" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16" s="62"/>
+      <c r="J16" s="19" t="e">
+        <f>IF(G16="X",VALUE(P6)+VALUE(U4),VALUE(P6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M16" s="63"/>
+      <c r="N16" s="63"/>
+      <c r="O16" s="63"/>
+      <c r="P16" s="63"/>
+      <c r="Q16" s="63"/>
+      <c r="R16" s="63"/>
+      <c r="S16" s="63"/>
+      <c r="T16" s="63"/>
     </row>
     <row r="17">
-      <c r="G17" s="62"/>
-      <c r="H17" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="I17" s="17"/>
-      <c r="J17" s="62"/>
-      <c r="M17" s="65"/>
-      <c r="N17" s="65"/>
-      <c r="O17" s="65"/>
-      <c r="P17" s="65"/>
-      <c r="Q17" s="65"/>
-      <c r="R17" s="65"/>
-      <c r="S17" s="65"/>
-      <c r="T17" s="65"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" s="16"/>
+      <c r="J17" s="19" t="e">
+        <f>IF(G17="X",VALUE(S6)+VALUE(U4),VALUE(S6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M17" s="63"/>
+      <c r="N17" s="63"/>
+      <c r="O17" s="63"/>
+      <c r="P17" s="63"/>
+      <c r="Q17" s="63"/>
+      <c r="R17" s="63"/>
+      <c r="S17" s="63"/>
+      <c r="T17" s="63"/>
     </row>
     <row r="18">
       <c r="B18" s="60" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C18" s="60"/>
       <c r="D18" s="60"/>
       <c r="E18" s="60"/>
-      <c r="G18" s="62"/>
+      <c r="G18" s="19"/>
       <c r="H18" s="14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I18" s="14"/>
-      <c r="J18" s="62"/>
-      <c r="M18" s="65"/>
-      <c r="N18" s="65"/>
-      <c r="O18" s="65"/>
-      <c r="P18" s="65"/>
-      <c r="Q18" s="65"/>
-      <c r="R18" s="65"/>
-      <c r="S18" s="65"/>
-      <c r="T18" s="65"/>
+      <c r="J18" s="19" t="e">
+        <f>IF(G18="X",VALUE(M6)+VALUE(U4),VALUE(M6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M18" s="63"/>
+      <c r="N18" s="63"/>
+      <c r="O18" s="63"/>
+      <c r="P18" s="63"/>
+      <c r="Q18" s="63"/>
+      <c r="R18" s="63"/>
+      <c r="S18" s="63"/>
+      <c r="T18" s="63"/>
     </row>
     <row r="19">
-      <c r="B19" s="65"/>
-      <c r="C19" s="65"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="65"/>
-      <c r="G19" s="62"/>
-      <c r="H19" s="64" t="s">
-        <v>56</v>
-      </c>
-      <c r="I19" s="64"/>
-      <c r="J19" s="62"/>
-      <c r="M19" s="65"/>
-      <c r="N19" s="65"/>
-      <c r="O19" s="65"/>
-      <c r="P19" s="65"/>
-      <c r="Q19" s="65"/>
-      <c r="R19" s="65"/>
-      <c r="S19" s="65"/>
-      <c r="T19" s="65"/>
+      <c r="B19" s="63"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
+      <c r="E19" s="63"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19" s="62"/>
+      <c r="J19" s="19" t="e">
+        <f>IF(G19="X",VALUE(P6)+VALUE(U4),VALUE(P6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M19" s="63"/>
+      <c r="N19" s="63"/>
+      <c r="O19" s="63"/>
+      <c r="P19" s="63"/>
+      <c r="Q19" s="63"/>
+      <c r="R19" s="63"/>
+      <c r="S19" s="63"/>
+      <c r="T19" s="63"/>
     </row>
     <row r="20">
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="G20" s="62"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="63"/>
+      <c r="G20" s="19"/>
       <c r="H20" s="14" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="I20" s="14"/>
-      <c r="J20" s="62"/>
-      <c r="M20" s="65"/>
-      <c r="N20" s="65"/>
-      <c r="O20" s="65"/>
-      <c r="P20" s="65"/>
-      <c r="Q20" s="65"/>
-      <c r="R20" s="65"/>
-      <c r="S20" s="65"/>
-      <c r="T20" s="65"/>
+      <c r="J20" s="19" t="e">
+        <f>IF(G20="X",VALUE(M6)+VALUE(U4),VALUE(M6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M20" s="63"/>
+      <c r="N20" s="63"/>
+      <c r="O20" s="63"/>
+      <c r="P20" s="63"/>
+      <c r="Q20" s="63"/>
+      <c r="R20" s="63"/>
+      <c r="S20" s="63"/>
+      <c r="T20" s="63"/>
     </row>
     <row r="21">
-      <c r="B21" s="65"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="65"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="64" t="s">
-        <v>58</v>
-      </c>
-      <c r="I21" s="64"/>
-      <c r="J21" s="62"/>
-      <c r="M21" s="65"/>
-      <c r="N21" s="65"/>
-      <c r="O21" s="65"/>
-      <c r="P21" s="65"/>
-      <c r="Q21" s="65"/>
-      <c r="R21" s="65"/>
-      <c r="S21" s="65"/>
-      <c r="T21" s="65"/>
+      <c r="B21" s="63"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="63"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="I21" s="62"/>
+      <c r="J21" s="19" t="e">
+        <f>IF(G21="X",VALUE(P6)+VALUE(U4),VALUE(P6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M21" s="63"/>
+      <c r="N21" s="63"/>
+      <c r="O21" s="63"/>
+      <c r="P21" s="63"/>
+      <c r="Q21" s="63"/>
+      <c r="R21" s="63"/>
+      <c r="S21" s="63"/>
+      <c r="T21" s="63"/>
     </row>
     <row r="22">
-      <c r="B22" s="65"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="65"/>
-      <c r="E22" s="65"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="I22" s="17"/>
-      <c r="J22" s="62"/>
-      <c r="M22" s="65"/>
-      <c r="N22" s="65"/>
-      <c r="O22" s="65"/>
-      <c r="P22" s="65"/>
-      <c r="Q22" s="65"/>
-      <c r="R22" s="65"/>
-      <c r="S22" s="65"/>
-      <c r="T22" s="65"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="63"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="I22" s="16"/>
+      <c r="J22" s="19" t="e">
+        <f>IF(G22="X",VALUE(S6)+VALUE(U4),VALUE(S6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M22" s="63"/>
+      <c r="N22" s="63"/>
+      <c r="O22" s="63"/>
+      <c r="P22" s="63"/>
+      <c r="Q22" s="63"/>
+      <c r="R22" s="63"/>
+      <c r="S22" s="63"/>
+      <c r="T22" s="63"/>
     </row>
     <row r="23">
-      <c r="B23" s="65"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="I23" s="17"/>
-      <c r="J23" s="62"/>
-      <c r="M23" s="65"/>
-      <c r="N23" s="65"/>
-      <c r="O23" s="65"/>
-      <c r="P23" s="65"/>
-      <c r="Q23" s="65"/>
-      <c r="R23" s="65"/>
-      <c r="S23" s="65"/>
-      <c r="T23" s="65"/>
+      <c r="B23" s="63"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="63"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="I23" s="16"/>
+      <c r="J23" s="19" t="e">
+        <f>IF(G23="X",VALUE(S6)+VALUE(U4),VALUE(S6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M23" s="63"/>
+      <c r="N23" s="63"/>
+      <c r="O23" s="63"/>
+      <c r="P23" s="63"/>
+      <c r="Q23" s="63"/>
+      <c r="R23" s="63"/>
+      <c r="S23" s="63"/>
+      <c r="T23" s="63"/>
     </row>
     <row r="24">
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="G24" s="62"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="63"/>
+      <c r="G24" s="19"/>
       <c r="H24" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I24" s="14"/>
-      <c r="J24" s="62"/>
-      <c r="M24" s="65"/>
-      <c r="N24" s="65"/>
-      <c r="O24" s="65"/>
-      <c r="P24" s="65"/>
-      <c r="Q24" s="65"/>
-      <c r="R24" s="65"/>
-      <c r="S24" s="65"/>
-      <c r="T24" s="65"/>
+      <c r="J24" s="19" t="e">
+        <f>IF(G24="X",VALUE(M6)+VALUE(U4),VALUE(M6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M24" s="63"/>
+      <c r="N24" s="63"/>
+      <c r="O24" s="63"/>
+      <c r="P24" s="63"/>
+      <c r="Q24" s="63"/>
+      <c r="R24" s="63"/>
+      <c r="S24" s="63"/>
+      <c r="T24" s="63"/>
     </row>
     <row r="25">
-      <c r="B25" s="65"/>
-      <c r="C25" s="65"/>
-      <c r="D25" s="65"/>
-      <c r="E25" s="65"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="63" t="s">
-        <v>62</v>
-      </c>
-      <c r="I25" s="63"/>
-      <c r="J25" s="62"/>
-      <c r="M25" s="65"/>
-      <c r="N25" s="65"/>
-      <c r="O25" s="65"/>
-      <c r="P25" s="65"/>
-      <c r="Q25" s="65"/>
-      <c r="R25" s="65"/>
-      <c r="S25" s="65"/>
-      <c r="T25" s="65"/>
+      <c r="B25" s="63"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="61" t="s">
+        <v>63</v>
+      </c>
+      <c r="I25" s="61"/>
+      <c r="J25" s="19" t="e">
+        <f>IF(G25="X",VALUE(G6)+VALUE(U4),VALUE(G6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M25" s="63"/>
+      <c r="N25" s="63"/>
+      <c r="O25" s="63"/>
+      <c r="P25" s="63"/>
+      <c r="Q25" s="63"/>
+      <c r="R25" s="63"/>
+      <c r="S25" s="63"/>
+      <c r="T25" s="63"/>
     </row>
     <row r="26">
-      <c r="B26" s="65"/>
-      <c r="C26" s="65"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="65"/>
-      <c r="G26" s="62"/>
-      <c r="H26" s="63" t="s">
-        <v>63</v>
-      </c>
-      <c r="I26" s="63"/>
-      <c r="J26" s="62"/>
-      <c r="M26" s="65"/>
-      <c r="N26" s="65"/>
-      <c r="O26" s="65"/>
-      <c r="P26" s="65"/>
-      <c r="Q26" s="65"/>
-      <c r="R26" s="65"/>
-      <c r="S26" s="65"/>
-      <c r="T26" s="65"/>
+      <c r="B26" s="63"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="I26" s="61"/>
+      <c r="J26" s="19" t="e">
+        <f>IF(G26="X",VALUE(G6)+VALUE(U4),VALUE(G6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M26" s="63"/>
+      <c r="N26" s="63"/>
+      <c r="O26" s="63"/>
+      <c r="P26" s="63"/>
+      <c r="Q26" s="63"/>
+      <c r="R26" s="63"/>
+      <c r="S26" s="63"/>
+      <c r="T26" s="63"/>
     </row>
     <row r="27">
-      <c r="B27" s="65"/>
-      <c r="C27" s="65"/>
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="64" t="s">
-        <v>64</v>
-      </c>
-      <c r="I27" s="64"/>
-      <c r="J27" s="62"/>
-      <c r="M27" s="65"/>
-      <c r="N27" s="65"/>
-      <c r="O27" s="65"/>
-      <c r="P27" s="65"/>
-      <c r="Q27" s="65"/>
-      <c r="R27" s="65"/>
-      <c r="S27" s="65"/>
-      <c r="T27" s="65"/>
+      <c r="B27" s="63"/>
+      <c r="C27" s="63"/>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="I27" s="54"/>
+      <c r="J27" s="19" t="e">
+        <f>IF(G27="X",VALUE(P6)+VALUE(U4),VALUE(P6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M27" s="63"/>
+      <c r="N27" s="63"/>
+      <c r="O27" s="63"/>
+      <c r="P27" s="63"/>
+      <c r="Q27" s="63"/>
+      <c r="R27" s="63"/>
+      <c r="S27" s="63"/>
+      <c r="T27" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="123">
@@ -2566,4 +2671,38 @@
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1"/>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>